<commit_message>
Cambios a la función de diccionario_rutas y eliminación de importaciones_mapas.py
</commit_message>
<xml_diff>
--- a/metodos_mixtos/rutas.xlsx
+++ b/metodos_mixtos/rutas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metodosmixtos.sharepoint.com/sites/MMC-General/Shared Documents/Programacion/funciones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metodosmixtos.sharepoint.com/sites/MMC-General/Shared Documents/Programacion/metodos-mixtos/metodos_mixtos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{066A9F54-7A76-F448-B9AB-44FB0538A963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9582D395-6584-3A47-BA4C-5FCD0CF14133}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{066A9F54-7A76-F448-B9AB-44FB0538A963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30ADE236-D088-F246-90A8-42A9992A08A4}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="21380" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25320" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="197">
   <si>
     <t>Key</t>
   </si>
@@ -343,162 +343,9 @@
     <t>descrip</t>
   </si>
   <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/registro_2021.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/Registro_2020_Noviembre.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 2/Monitoreo_UNODC/Lotes_Comprometidos_PNIS.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/Lotes_PNIS_ErradicacionTotal_11112020.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/monitoreo_pagos.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 2/Monitoreo_UNODC/Lotes_PNIS_pagos.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 2/Monitoreo_UNODC/Vdas_PNIS.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_ART_10092019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_DANE_10092019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_OtrasDA_10092019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_PNIS_10092019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/emf/EMF_2016_2020_Completo/EMF_2016_2020_Completo.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/zonas_futuro/zonas_futuro.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Conflicto/map/map_2016_2020.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Conflicto/map/map_octubre_31_2020.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/mineria_evoa/EVOA2019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/mineria_evoa/evoa_veredas.xlsx</t>
-  </si>
-  <si>
     <t>geoinfo/Colombia/Conflicto/grupos_armados/grupos.shp</t>
   </si>
   <si>
-    <t>MMC - General - geoinfo/Colombia/ADMINISTRATIVO/colombia.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/CRVeredas_2017.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/CRVeredas_2020/CRVeredas_2020.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/ADMINISTRATIVO/VRDS_MPIO_POLITICO.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/ADMINISTRATIVO/MGN_MPIO_POLITICO.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/ADMINISTRATIVO/VRDS_MPIO_INDEX.csv</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/ADMINISTRATIVO/MGN_DPTO_POLITICO.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/DIVIPOLA_MUN.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/Parques_Nacionales_Naturales.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/Resguardos_Indigenas.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/Consejos_comunitarios.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/bosques/runap2/runap2Polygon.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/bosques/Humedales_RAMSAR_Agosto_2018/Humedales_RAMSAR_Agosto_2018.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/bosques/Paramos_Delimitados_Junio_2020/Paramos_Delimitados_Junio_2020.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/Sustracciones_Definitivas_Ley2_marzo_2021/Sustracciones_Definitivas_Ley2_marzo_2021.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/Zonificacion_Ley2_julio_2022/Zonificacion_Ley2_julio_2022.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/Reserva_Ley2_marzo_2021/Reserva_Ley2_marzo_2021.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Territoriales/jurisdicciones_especiales.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/ADMINISTRATIVO/MGN2020_URB_AREA_CENSAL/MGN_URB_AREA_CENSAL.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/municipales/panel_municipales_pgn.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Geografia/rios/Rios_principales.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Infraestructura/Via/Via.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/bases_tania/listado_aero_aerocivil.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/bases_tania/listado_aero_pub_priv.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Agro/Palma/Lotes_18022019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/bases/base_veredas/base_veredas.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/base_veredas/vrds</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/CNPV/ShapefileMGN_ANM_SECCION_RURAL/MGN_ANM_SECCION_RURAL.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/CNPV/ShapefileMGN_ANM_SECCION_RURAL/tabla_referencia_cnpv.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/CNA/Total_nacional(csv)/S01_15(Unidad_productora).csv</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/CNA/Total_nacional(csv)/S06A(Cultivos).csv</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/CNA/Total_nacional(csv)/S09(Maquinaria_uso_agropecuario).csv</t>
-  </si>
-  <si>
-    <t>MMC - General - Programacion/bases/CNA/Total_nacional(csv)/S10(Construcciones_uso_agropecuario).csv</t>
-  </si>
-  <si>
     <t>LFP_compartido/sistemas_informacion/Insumos TetraTech/Piloto Modulo de Beneficiarios/Bases_Estandarizadas/Fisos Ovejas.xlsx</t>
   </si>
   <si>
@@ -511,115 +358,259 @@
     <t>LFP_compartido/sistemas_informacion/Insumos TetraTech/Piloto Modulo de Beneficiarios/Bases_Estandarizadas/FormalizadosLRDP.xlsx</t>
   </si>
   <si>
-    <t>MMC - General - Programacion/bases/municipales/27-01-2021 Caracterización municipios.xlsx</t>
-  </si>
-  <si>
     <t>LFP_compartido/cooperacion/cooperacion_municipal.xlsx</t>
   </si>
   <si>
-    <t>MMC - General - geoinfo/Colombia/delitos/Base/Delitos.dta</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/delitos/Base/2016-2019 Estupefacientes.dta</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/delitos/Base/2016-2019 Armas.dta</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/delitos/Base/2016-2019 Capturas.dta</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/socioeconomicas/proyeccion_poblacion.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/deforestacion/forest_loss_mpios.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/deforestacion/forest_loss_veredas.xlsx</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2001.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2002.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2003.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2004.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2005.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2006.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2007.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2008.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2009.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2010.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2011.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2012.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2013.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2014.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2015.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2016.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2017.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2018.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2019.shp</t>
-  </si>
-  <si>
-    <t>MMC - General - geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2020.shp</t>
-  </si>
-  <si>
     <t>access_market</t>
   </si>
   <si>
-    <t>MMC - General - geoinfo/Internacionales/travel_time_to_cities_11.tif</t>
-  </si>
-  <si>
-    <t>pib</t>
-  </si>
-  <si>
     <t>socioeconomico</t>
   </si>
   <si>
-    <t>MMC - General - FIDA/Data/PIB_per_capita/GDP_PPP_1990_2015_5arcmin_v2.nc</t>
-  </si>
-  <si>
     <t>inflation_usa</t>
   </si>
   <si>
-    <t>MMC - General - Programacion/funciones/FPCPITOTLZGUSA.csv</t>
+    <t>geoinfo/Respuesta DCSI 3/Registro_2020_Noviembre.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/registro_2021.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 2/Monitoreo_UNODC/Lotes_Comprometidos_PNIS.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/Lotes_PNIS_ErradicacionTotal_11112020.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/monitoreo_pagos.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 2/Monitoreo_UNODC/Lotes_PNIS_pagos.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 2/Monitoreo_UNODC/Vdas_PNIS.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_ART_10092019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_DANE_10092019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_OtrasDA_10092019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Respuesta DCSI 3/Vdas_AcuerdosColectivos_PNIS_10092019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/emf/EMF_2016_2020_Completo/EMF_2016_2020_Completo.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/zonas_futuro/zonas_futuro.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Conflicto/map/map_2016_2020.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Conflicto/map/map_octubre_31_2020.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/mineria_evoa/EVOA2019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/mineria_evoa/evoa_veredas.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/ADMINISTRATIVO/colombia.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/CRVeredas_2017.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/CRVeredas_2020/CRVeredas_2020.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/ADMINISTRATIVO/VRDS_MPIO_POLITICO.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/ADMINISTRATIVO/MGN_MPIO_POLITICO.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/ADMINISTRATIVO/VRDS_MPIO_INDEX.csv</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/ADMINISTRATIVO/MGN_DPTO_POLITICO.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/DIVIPOLA_MUN.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/Parques_Nacionales_Naturales.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/Resguardos_Indigenas.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/Consejos_comunitarios.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/bosques/runap2/runap2Polygon.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/bosques/Humedales_RAMSAR_Agosto_2018/Humedales_RAMSAR_Agosto_2018.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/bosques/Paramos_Delimitados_Junio_2020/Paramos_Delimitados_Junio_2020.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/Sustracciones_Definitivas_Ley2_marzo_2021/Sustracciones_Definitivas_Ley2_marzo_2021.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/Zonificacion_Ley2_julio_2022/Zonificacion_Ley2_julio_2022.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/Reserva_Ley2_marzo_2021/Reserva_Ley2_marzo_2021.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Territoriales/jurisdicciones_especiales.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/ADMINISTRATIVO/MGN2020_URB_AREA_CENSAL/MGN_URB_AREA_CENSAL.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Geografia/rios/Rios_principales.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Infraestructura/Via/Via.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/bases_tania/listado_aero_aerocivil.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/bases_tania/listado_aero_pub_priv.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Agro/Palma/Lotes_18022019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/bases/base_veredas/base_veredas.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/delitos/Base/Delitos.dta</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/delitos/Base/2016-2019 Estupefacientes.dta</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/delitos/Base/2016-2019 Armas.dta</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/delitos/Base/2016-2019 Capturas.dta</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/socioeconomicas/proyeccion_poblacion.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/deforestacion/forest_loss_mpios.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/deforestacion/forest_loss_veredas.xlsx</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2001.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2002.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2003.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2004.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2005.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2006.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2007.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2008.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2009.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2010.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2011.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2012.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2013.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2014.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2015.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2016.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2017.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2018.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2019.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Colombia/Narcotrafico/densidad_coca/Densidad_Cultivos_Ilícitos_2020.shp</t>
+  </si>
+  <si>
+    <t>geoinfo/Internacionales/travel_time_to_cities_11.tif</t>
+  </si>
+  <si>
+    <t>programacion/bases/municipales/panel_municipales_pgn.xlsx</t>
+  </si>
+  <si>
+    <t>programacion/bases/base_veredas/vrds</t>
+  </si>
+  <si>
+    <t>programacion/bases/CNPV/ShapefileMGN_ANM_SECCION_RURAL/MGN_ANM_SECCION_RURAL.shp</t>
+  </si>
+  <si>
+    <t>programacion/bases/CNPV/ShapefileMGN_ANM_SECCION_RURAL/tabla_referencia_cnpv.xlsx</t>
+  </si>
+  <si>
+    <t>programacion/bases/CNA/Total_nacional(csv)/S01_15(Unidad_productora).csv</t>
+  </si>
+  <si>
+    <t>programacion/bases/CNA/Total_nacional(csv)/S06A(Cultivos).csv</t>
+  </si>
+  <si>
+    <t>programacion/bases/CNA/Total_nacional(csv)/S09(Maquinaria_uso_agropecuario).csv</t>
+  </si>
+  <si>
+    <t>programacion/bases/CNA/Total_nacional(csv)/S10(Construcciones_uso_agropecuario).csv</t>
+  </si>
+  <si>
+    <t>programacion/bases/municipales/27-01-2021 Caracterización municipios.xlsx</t>
+  </si>
+  <si>
+    <t>programacion/funciones/FPCPITOTLZGUSA.csv</t>
   </si>
 </sst>
 </file>
@@ -994,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1028,7 +1019,7 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1039,7 +1030,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1050,7 +1041,7 @@
         <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1061,7 +1052,7 @@
         <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1072,7 +1063,7 @@
         <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1083,7 +1074,7 @@
         <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1094,7 +1085,7 @@
         <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1105,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1116,7 +1107,7 @@
         <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1127,7 +1118,7 @@
         <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1138,7 +1129,7 @@
         <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1149,7 +1140,7 @@
         <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1160,7 +1151,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1171,7 +1162,7 @@
         <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,7 +1173,7 @@
         <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1193,7 +1184,7 @@
         <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1204,7 +1195,7 @@
         <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1215,7 +1206,7 @@
         <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1226,7 +1217,7 @@
         <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1237,7 +1228,7 @@
         <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1248,7 +1239,7 @@
         <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1259,7 +1250,7 @@
         <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1270,7 +1261,7 @@
         <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1281,7 +1272,7 @@
         <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1292,7 +1283,7 @@
         <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1303,7 +1294,7 @@
         <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1314,7 +1305,7 @@
         <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1325,7 +1316,7 @@
         <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,7 +1327,7 @@
         <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1347,7 +1338,7 @@
         <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1358,7 +1349,7 @@
         <v>95</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1369,7 +1360,7 @@
         <v>95</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1380,7 +1371,7 @@
         <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1391,7 +1382,7 @@
         <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1402,7 +1393,7 @@
         <v>95</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1413,7 +1404,7 @@
         <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1424,7 +1415,7 @@
         <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1435,7 +1426,7 @@
         <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1446,7 +1437,7 @@
         <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1457,7 +1448,7 @@
         <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1468,7 +1459,7 @@
         <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1479,7 +1470,7 @@
         <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,7 +1481,7 @@
         <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1501,7 +1492,7 @@
         <v>101</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1512,7 +1503,7 @@
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1523,7 +1514,7 @@
         <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1534,7 +1525,7 @@
         <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1545,7 +1536,7 @@
         <v>65</v>
       </c>
       <c r="D49" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1556,7 +1547,7 @@
         <v>65</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1567,7 +1558,7 @@
         <v>101</v>
       </c>
       <c r="D51" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1578,7 +1569,7 @@
         <v>101</v>
       </c>
       <c r="D52" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1589,7 +1580,7 @@
         <v>101</v>
       </c>
       <c r="D53" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1600,7 +1591,7 @@
         <v>102</v>
       </c>
       <c r="D54" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1611,7 +1602,7 @@
         <v>102</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1622,7 +1613,7 @@
         <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1633,7 +1624,7 @@
         <v>102</v>
       </c>
       <c r="D57" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1644,7 +1635,7 @@
         <v>103</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1655,7 +1646,7 @@
         <v>104</v>
       </c>
       <c r="D59" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1666,7 +1657,7 @@
         <v>105</v>
       </c>
       <c r="D60" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1677,7 +1668,7 @@
         <v>105</v>
       </c>
       <c r="D61" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1688,7 +1679,7 @@
         <v>105</v>
       </c>
       <c r="D62" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1699,7 +1690,7 @@
         <v>105</v>
       </c>
       <c r="D63" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1710,7 +1701,7 @@
         <v>103</v>
       </c>
       <c r="D64" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1721,7 +1712,7 @@
         <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1732,7 +1723,7 @@
         <v>95</v>
       </c>
       <c r="D66" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1743,7 +1734,7 @@
         <v>95</v>
       </c>
       <c r="D67" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1754,7 +1745,7 @@
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1765,7 +1756,7 @@
         <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1776,7 +1767,7 @@
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1787,7 +1778,7 @@
         <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1798,7 +1789,7 @@
         <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1809,7 +1800,7 @@
         <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1820,7 +1811,7 @@
         <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1831,7 +1822,7 @@
         <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1842,7 +1833,7 @@
         <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1853,7 +1844,7 @@
         <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1864,7 +1855,7 @@
         <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1875,7 +1866,7 @@
         <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1886,7 +1877,7 @@
         <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1897,7 +1888,7 @@
         <v>9</v>
       </c>
       <c r="D81" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -1908,7 +1899,7 @@
         <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1919,7 +1910,7 @@
         <v>9</v>
       </c>
       <c r="D83" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1930,7 +1921,7 @@
         <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1941,7 +1932,7 @@
         <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1952,7 +1943,7 @@
         <v>9</v>
       </c>
       <c r="D86" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1963,40 +1954,29 @@
         <v>9</v>
       </c>
       <c r="D87" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
         <v>100</v>
       </c>
       <c r="D88" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>195</v>
+        <v>115</v>
       </c>
       <c r="B89" t="s">
+        <v>114</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>198</v>
-      </c>
-      <c r="B90" t="s">
-        <v>196</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2016,6 +1996,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D921533D1D68634C86DF2AE5A7B8FD15" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1c3c32f3d82fd82e6afb0ecd9b71d984">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fda77056-5abb-4cef-9e5f-e441f657d77f" xmlns:ns3="6a07986a-6cf0-42f6-9741-92984a6f5818" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e853ef6ac2a0b4566ae3509c88f9c512" ns2:_="" ns3:_="">
     <xsd:import namespace="fda77056-5abb-4cef-9e5f-e441f657d77f"/>
@@ -2250,33 +2239,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D58E4C-CC55-412F-BFF0-5F7107827CFE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6a07986a-6cf0-42f6-9741-92984a6f5818"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6a07986a-6cf0-42f6-9741-92984a6f5818"/>
     <ds:schemaRef ds:uri="fda77056-5abb-4cef-9e5f-e441f657d77f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{096126C8-0308-42BB-BA35-E40E95801B17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F961D3C-C213-4020-AFFC-E3B65C7F7D6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2293,12 +2281,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{096126C8-0308-42BB-BA35-E40E95801B17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>